<commit_message>
Result and evaluation part of thesis
</commit_message>
<xml_diff>
--- a/thesis/Evaluation.xlsx
+++ b/thesis/Evaluation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="25">
   <si>
     <t>1280 x 720</t>
   </si>
@@ -88,12 +88,18 @@
   </si>
   <si>
     <t>Bytes received</t>
+  </si>
+  <si>
+    <t>up to 30 Mb/s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -188,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -207,6 +213,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -512,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:H28"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -521,7 +530,7 @@
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="3" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="8" width="13.5703125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
@@ -933,7 +942,7 @@
         <v>8</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="15" x14ac:dyDescent="0.25">
@@ -974,16 +983,16 @@
       <c r="D29" s="6">
         <v>30</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="10">
         <v>1.5</v>
       </c>
-      <c r="F29" s="5">
-        <v>3.2</v>
-      </c>
-      <c r="G29" s="5">
+      <c r="F29" s="10">
+        <v>3</v>
+      </c>
+      <c r="G29" s="10">
         <v>3.5</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29" s="10">
         <v>3.8</v>
       </c>
     </row>
@@ -994,17 +1003,17 @@
       <c r="D30" s="6">
         <v>30</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="10">
         <v>3.9</v>
       </c>
-      <c r="F30" s="5">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="G30" s="5">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="H30" s="5">
+      <c r="F30" s="10">
+        <v>4.3</v>
+      </c>
+      <c r="G30" s="10">
         <v>4.7</v>
+      </c>
+      <c r="H30" s="10">
+        <v>4.8</v>
       </c>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.2">
@@ -1014,17 +1023,17 @@
       <c r="D31" s="6">
         <v>30</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="10">
         <v>3.7</v>
       </c>
-      <c r="F31" s="5">
-        <v>3.7</v>
-      </c>
-      <c r="G31" s="5">
-        <v>4</v>
-      </c>
-      <c r="H31" s="5">
-        <v>4.0999999999999996</v>
+      <c r="F31" s="10">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G31" s="10">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H31" s="10">
+        <v>4.5999999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -1035,6 +1044,7 @@
     <mergeCell ref="E28:H28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>